<commit_message>
Updating Legaledge files, XML samples and mapping.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl/hawaii/LegalEdge.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl/hawaii/LegalEdge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jim/git/OJB/main/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl/hawaii/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B892A815-A8C0-BD46-8AE3-A0DA86BD8C55}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{53E68030-D481-9741-B7FE-C4CDFC90FD9C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31160" yWindow="800" windowWidth="16720" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36340" yWindow="1060" windowWidth="16720" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Filing Decision" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="125">
   <si>
     <t>Defendant</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Case Number</t>
   </si>
   <si>
-    <t>Disposition</t>
-  </si>
-  <si>
     <t>Case Open Indicator</t>
   </si>
   <si>
@@ -78,15 +75,9 @@
     <t>Defendant Names</t>
   </si>
   <si>
-    <t>Offense Category</t>
-  </si>
-  <si>
     <t>Severity?</t>
   </si>
   <si>
-    <t>Case Weight Indicator</t>
-  </si>
-  <si>
     <t>Definition?</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t>Case Comments</t>
   </si>
   <si>
-    <t>Subject/Defendant</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -298,6 +286,120 @@
   </si>
   <si>
     <t>Date Expires</t>
+  </si>
+  <si>
+    <t>Incidents</t>
+  </si>
+  <si>
+    <t>DR Number</t>
+  </si>
+  <si>
+    <t>Incident Date</t>
+  </si>
+  <si>
+    <t>Report Date</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Weapon Indicator</t>
+  </si>
+  <si>
+    <t>Arresting Agency Name</t>
+  </si>
+  <si>
+    <t>Arresting Officer</t>
+  </si>
+  <si>
+    <t>Incident Comment</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Offers</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Facts</t>
+  </si>
+  <si>
+    <t>File Location</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Evidence</t>
+  </si>
+  <si>
+    <t>Related Cases</t>
+  </si>
+  <si>
+    <t>Forfeiture Cases</t>
+  </si>
+  <si>
+    <t>Case Notes</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Created By</t>
+  </si>
+  <si>
+    <t>File Attachment</t>
+  </si>
+  <si>
+    <t>Quick Templates</t>
+  </si>
+  <si>
+    <t>Open/Closed</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>CR200-034</t>
+  </si>
+  <si>
+    <t>Holbrook Justice Court</t>
+  </si>
+  <si>
+    <t>03-2345</t>
+  </si>
+  <si>
+    <t>06-06-2004</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>Crime (Offense) Category</t>
+  </si>
+  <si>
+    <t>Case Weight</t>
+  </si>
+  <si>
+    <t>Definition? Values?</t>
+  </si>
+  <si>
+    <t>Case Disposition</t>
+  </si>
+  <si>
+    <t>Subject/Defendant(s)</t>
   </si>
 </sst>
 </file>
@@ -1776,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1790,18 +1892,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16">
       <c r="A1" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1809,61 +1911,82 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C7" s="12" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="C8" s="12" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1871,93 +1994,96 @@
         <v>5</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A21" s="9"/>
       <c r="B21" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C21" s="13"/>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A23" s="9"/>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C23" s="13"/>
     </row>
     <row r="24" spans="1:3">
       <c r="B24" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A25" s="9"/>
       <c r="B25" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" s="13"/>
     </row>
@@ -1968,7 +2094,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>4</v>
@@ -1976,46 +2102,46 @@
     </row>
     <row r="29" spans="1:3">
       <c r="B29" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C29" s="15"/>
     </row>
     <row r="30" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A30" s="14"/>
       <c r="B30" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C30" s="13"/>
     </row>
     <row r="31" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A31" s="9"/>
       <c r="B31" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A32" s="9"/>
       <c r="B32" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A33" s="9"/>
       <c r="B33" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A34" s="9"/>
       <c r="B34" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C34" s="13"/>
     </row>
@@ -2026,24 +2152,24 @@
     </row>
     <row r="36" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A36" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C36" s="13"/>
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A37" s="9"/>
       <c r="B37" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C37" s="13"/>
     </row>
     <row r="38" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A38" s="9"/>
       <c r="B38" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C38" s="13"/>
     </row>
@@ -2066,7 +2192,7 @@
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A42" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>3</v>
@@ -2076,61 +2202,61 @@
     <row r="43" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A43" s="9"/>
       <c r="B43" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C43" s="13"/>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="7"/>
       <c r="B45" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="7"/>
       <c r="B46" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="7"/>
       <c r="B47" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="7"/>
       <c r="B48" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="7"/>
       <c r="B49" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A50" s="8"/>
       <c r="B50" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C50" s="13"/>
     </row>
@@ -2141,7 +2267,7 @@
     </row>
     <row r="52" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A52" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>1</v>
@@ -2155,10 +2281,10 @@
     </row>
     <row r="54" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A54" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C54" s="13"/>
     </row>
@@ -2169,69 +2295,69 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="7"/>
       <c r="B57" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="7"/>
       <c r="B58" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="7"/>
       <c r="B59" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="14"/>
       <c r="B60" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A61" s="9"/>
       <c r="B61" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C61" s="13"/>
     </row>
     <row r="62" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A62" s="9"/>
       <c r="B62" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C62" s="13"/>
     </row>
     <row r="63" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A63" s="9"/>
       <c r="B63" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C63" s="13"/>
     </row>
     <row r="64" spans="1:3">
       <c r="B64" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2241,67 +2367,67 @@
     </row>
     <row r="66" spans="1:3">
       <c r="B66" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="B67" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A69" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C69" s="13"/>
     </row>
     <row r="70" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A70" s="9"/>
       <c r="B70" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C70" s="13"/>
     </row>
     <row r="71" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A71" s="9"/>
       <c r="B71" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A72" s="9"/>
       <c r="B72" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C72" s="13"/>
     </row>
     <row r="73" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A73" s="9"/>
       <c r="B73" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C73" s="13"/>
     </row>
     <row r="74" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A74" s="9"/>
       <c r="B74" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C74" s="13"/>
     </row>
     <row r="75" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A75" s="8"/>
       <c r="B75" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C75" s="13"/>
     </row>
@@ -2312,11 +2438,11 @@
     </row>
     <row r="77" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A77" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="2" customFormat="1" ht="14">
@@ -2326,44 +2452,44 @@
     </row>
     <row r="79" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A79" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A80" s="9"/>
       <c r="B80" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C80" s="13"/>
     </row>
     <row r="81" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A81" s="9"/>
       <c r="B81" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C81" s="13"/>
     </row>
     <row r="82" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A82" s="9"/>
       <c r="B82" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C82" s="13"/>
     </row>
     <row r="83" spans="1:3">
       <c r="B83" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="B84" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="1:3" s="2" customFormat="1" ht="14">
@@ -2372,43 +2498,61 @@
       <c r="C85" s="13"/>
     </row>
     <row r="86" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A86" s="9"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="C86" s="13"/>
     </row>
     <row r="87" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A87" s="9"/>
-      <c r="B87" s="4"/>
+      <c r="B87" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="C87" s="13"/>
     </row>
     <row r="88" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A88" s="9"/>
-      <c r="B88" s="4"/>
+      <c r="B88" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="C88" s="13"/>
     </row>
     <row r="89" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A89" s="9"/>
-      <c r="B89" s="4"/>
+      <c r="B89" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="C89" s="13"/>
     </row>
     <row r="90" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A90" s="9"/>
-      <c r="B90" s="4"/>
+      <c r="B90" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="C90" s="13"/>
     </row>
     <row r="91" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A91" s="9"/>
-      <c r="B91" s="4"/>
+      <c r="B91" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="C91" s="13"/>
     </row>
     <row r="92" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A92" s="9"/>
-      <c r="B92" s="4"/>
+      <c r="B92" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="C92" s="13"/>
     </row>
     <row r="93" spans="1:3" s="2" customFormat="1" ht="14">
       <c r="A93" s="9"/>
-      <c r="B93" s="4"/>
+      <c r="B93" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="C93" s="13"/>
     </row>
     <row r="94" spans="1:3" s="2" customFormat="1" ht="14">
@@ -2417,63 +2561,108 @@
       <c r="C94" s="13"/>
     </row>
     <row r="95" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A95" s="9"/>
+      <c r="A95" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="B95" s="4"/>
       <c r="C95" s="13"/>
     </row>
     <row r="96" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A96" s="9"/>
+      <c r="A96" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="B96" s="4"/>
       <c r="C96" s="13"/>
     </row>
     <row r="97" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A97" s="9"/>
+      <c r="A97" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="B97" s="4"/>
       <c r="C97" s="13"/>
     </row>
     <row r="98" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A98" s="9"/>
+      <c r="A98" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="B98" s="4"/>
       <c r="C98" s="13"/>
     </row>
     <row r="99" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A99" s="9"/>
+      <c r="A99" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="B99" s="4"/>
       <c r="C99" s="13"/>
     </row>
     <row r="100" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A100" s="9"/>
+      <c r="A100" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="B100" s="4"/>
       <c r="C100" s="13"/>
     </row>
     <row r="101" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A101" s="9"/>
+      <c r="A101" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="B101" s="4"/>
       <c r="C101" s="13"/>
     </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="103" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A103" s="9"/>
+      <c r="A103" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="B103" s="4"/>
       <c r="C103" s="13"/>
     </row>
     <row r="104" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A104" s="9"/>
+      <c r="A104" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="B104" s="4"/>
       <c r="C104" s="13"/>
     </row>
     <row r="105" spans="1:3" s="2" customFormat="1" ht="14">
-      <c r="A105" s="9"/>
-      <c r="B105" s="4"/>
+      <c r="A105" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="C105" s="13"/>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="B106" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="7"/>
+      <c r="B107" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="10"/>
+      <c r="B108" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="8"/>
+      <c r="A110" s="8" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="8"/>

</xml_diff>